<commit_message>
setting up in mac
</commit_message>
<xml_diff>
--- a/not_in_warehouses_warehouse.xlsx
+++ b/not_in_warehouses_warehouse.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,6 +447,20 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Katha no 461 100 7, Comprised of Converted Survey No 100 4,</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>SY  No  99 1, Aduru Village,</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>